<commit_message>
Fer is love... Fer is Life... :heart:
</commit_message>
<xml_diff>
--- a/Project documents/elaboration-phase/20161006_modeldictionary.xlsx
+++ b/Project documents/elaboration-phase/20161006_modeldictionary.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\1-school\jaar-2\barroc-it-groep-5\Project documents\elaboration-phase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\barrocit\barroc-it-groep-5\Project documents\elaboration-phase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="82">
   <si>
     <t>Kandidaat klasse</t>
   </si>
@@ -216,13 +216,67 @@
   </si>
   <si>
     <t>ja</t>
+  </si>
+  <si>
+    <t>Barroc-IT is the company that will use this application for better communication</t>
+  </si>
+  <si>
+    <t>When a customer is registered and accepted, it can ask the development department to start a project. The project can be assigned to a customer and will get a project status which will show to current state of the project</t>
+  </si>
+  <si>
+    <t>Maintenance is a task the development department had. If the application they made needs support, they will provide it. The customer needs a maintenance contract to get access to this support</t>
+  </si>
+  <si>
+    <t>The Development role is one of the roles within the application</t>
+  </si>
+  <si>
+    <t>Invoices can be made within the application itself and can be assigned to customers. After that the quotation can be send to a customer so he can pay to bill. After the payment, the invoice will be set to "paid"</t>
+  </si>
+  <si>
+    <t>The finance role is one of the roles within the application</t>
+  </si>
+  <si>
+    <t>The conact date is a attribute at the appointments section. The user can see when the appointment took place here</t>
+  </si>
+  <si>
+    <t>An appointment can be assigned to a customer. If the user of the application wants to see threw a history of appointments of a customer he can do so</t>
+  </si>
+  <si>
+    <t>The offerstatus is something for the customer to see if his offer is accpted or denied</t>
+  </si>
+  <si>
+    <t>A customer has a company name attatched to it. This makes the customer unique towards the others</t>
+  </si>
+  <si>
+    <t>The database is the storage system for this application. All the data can be found here</t>
+  </si>
+  <si>
+    <t>Quotations can be made in the application itself and can be assigned and send to customers.</t>
+  </si>
+  <si>
+    <t>A customer is an object in the application. Custommers can have action projects or bills they need to pay</t>
+  </si>
+  <si>
+    <t>The sales role is one of the roles within the application</t>
+  </si>
+  <si>
+    <t>Departments will each get a different role in the application. One may be able to edit more data then the other</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Class type</t>
+  </si>
+  <si>
+    <t>Class</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +294,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,6 +471,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H66"/>
+  <dimension ref="B2:H72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,39 +1412,203 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B58" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B59" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="B60" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B61" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="F61" s="6"/>
       <c r="G61" s="16"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B62" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="F62" s="6"/>
       <c r="G62" s="16"/>
       <c r="H62" s="6"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B63" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="F63" s="6"/>
       <c r="G63" s="16"/>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B64" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="F64" s="6"/>
       <c r="G64" s="16"/>
       <c r="H64" s="6"/>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="F65" s="6"/>
       <c r="G65" s="16"/>
       <c r="H65" s="6"/>
     </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="B66" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="F66" s="6"/>
       <c r="G66" s="16"/>
       <c r="H66" s="6"/>
     </row>
+    <row r="67" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B69" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B70" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B71" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B72" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D42 D43:D54 D55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D55">
       <formula1>"Redundant,Irrelevant,Vaag,Niet kwantificeerbaar,Attribuut,Operatie"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>